<commit_message>
[excel] - [`csv(file,worksheet,range,output)`]: support multiple ranges.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/xml-showcase.xlsx
+++ b/src/test/resources/showcase/artifact/script/xml-showcase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EF300B-BCFC-3B44-A6BC-3A6CAB4EEEF9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79601FB-A533-384D-BC8E-7D344E0A4B86}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10960" windowWidth="51200" windowHeight="21040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20560" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -1531,40 +1531,10 @@
     <t>English,Spanish,German</t>
   </si>
   <si>
-    <t>[XML(${test1.file}) =&gt; 
- update-attribute(//book[@id='bk101'],id,bk999)
-]</t>
-  </si>
-  <si>
-    <t>[XML(${test1.file}) =&gt; 
- update-attribute(//book[@id='bk101'],id,)
-]</t>
-  </si>
-  <si>
-    <t>[XML(${test1.file}) =&gt; 
- attribute(//book[@id='bk110'],favorite)
-]</t>
-  </si>
-  <si>
     <t>get content</t>
   </si>
   <si>
     <t>Microsoft's .NET initiative is explored in detail in this deep programmer's reference.</t>
-  </si>
-  <si>
-    <t>[XML(${test1.file}) =&gt; 
- attribute(//book[contains(@id\,'bk11'\)],language)
-]</t>
-  </si>
-  <si>
-    <t>[XML(${test1.file}) =&gt; 
- content(//book[@id='bk110']/description)
-]</t>
-  </si>
-  <si>
-    <t>[XML(${test1.file}) =&gt; 
- content(//book[@language!='']/price)
-]</t>
   </si>
   <si>
     <t>36.95,36.95,49.95</t>
@@ -1602,6 +1572,24 @@
   </si>
   <si>
     <t>[XML(${test1.file}) =&gt; remove(//book[@id='bk104'])]</t>
+  </si>
+  <si>
+    <t>[XML(${test1.file}) =&gt; content(//book[@language!='']/price)]</t>
+  </si>
+  <si>
+    <t>[XML(${test1.file}) =&gt; content(//book[@id='bk110']/description)]</t>
+  </si>
+  <si>
+    <t>[XML(${test1.file}) =&gt; attribute(//book[@id='bk110'],favorite)]</t>
+  </si>
+  <si>
+    <t>[XML(${test1.file}) =&gt; attribute(//book[contains(@id\,'bk11'\)],language)]</t>
+  </si>
+  <si>
+    <t>[XML(${test1.file}) =&gt; update-attribute(//book[@id='bk101'],id,)]</t>
+  </si>
+  <si>
+    <t>[XML(${test1.file}) =&gt; update-attribute(//book[@id='bk101'],id,bk999)]</t>
   </si>
 </sst>
 </file>
@@ -1771,7 +1759,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1877,11 +1865,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1912,10 +1900,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3884,9 +3868,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3896,7 +3880,7 @@
     <col min="3" max="3" width="10.83203125" style="14" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="44.1640625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="32.6640625" style="10" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="88.5" style="10" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="94.83203125" style="10" customWidth="1" collapsed="1"/>
     <col min="7" max="9" width="18.33203125" style="10" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="18.33203125" style="23" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="1.6640625" style="11" customWidth="1" collapsed="1"/>
@@ -4022,7 +4006,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="31" t="s">
         <v>475</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -4241,11 +4225,11 @@
       <c r="N12" s="15"/>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="1:15" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="40" t="s">
+    <row r="13" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="31" t="s">
         <v>476</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30" t="s">
         <v>478</v>
       </c>
       <c r="C13" s="13" t="s">
@@ -4257,8 +4241,8 @@
       <c r="E13" s="10" t="s">
         <v>477</v>
       </c>
-      <c r="F13" s="30" t="s">
-        <v>489</v>
+      <c r="F13" s="22" t="s">
+        <v>507</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -4295,7 +4279,7 @@
       <c r="N14" s="15"/>
       <c r="O14" s="3"/>
     </row>
-    <row r="15" spans="1:15" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="29" t="s">
         <v>483</v>
@@ -4309,8 +4293,8 @@
       <c r="E15" s="10" t="s">
         <v>477</v>
       </c>
-      <c r="F15" s="30" t="s">
-        <v>490</v>
+      <c r="F15" s="22" t="s">
+        <v>506</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -4401,9 +4385,9 @@
       <c r="N18" s="15"/>
       <c r="O18" s="3"/>
     </row>
-    <row r="19" spans="1:15" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="30" t="s">
         <v>486</v>
       </c>
       <c r="C19" s="28" t="s">
@@ -4415,8 +4399,8 @@
       <c r="E19" s="27" t="s">
         <v>487</v>
       </c>
-      <c r="F19" s="30" t="s">
-        <v>491</v>
+      <c r="F19" s="22" t="s">
+        <v>504</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -4428,7 +4412,7 @@
       <c r="N19" s="15"/>
       <c r="O19" s="3"/>
     </row>
-    <row r="20" spans="1:15" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="28" t="s">
@@ -4441,7 +4425,7 @@
         <v>488</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="G20" s="27" t="s">
         <v>487</v>
@@ -4457,8 +4441,8 @@
     </row>
     <row r="21" spans="1:15" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
-      <c r="B21" s="40" t="s">
-        <v>492</v>
+      <c r="B21" s="31" t="s">
+        <v>489</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>13</v>
@@ -4467,10 +4451,10 @@
         <v>336</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
@@ -4482,7 +4466,7 @@
       <c r="N21" s="15"/>
       <c r="O21" s="3"/>
     </row>
-    <row r="22" spans="1:15" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="13" t="s">
@@ -4492,10 +4476,10 @@
         <v>15</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>487</v>
@@ -4511,8 +4495,8 @@
     </row>
     <row r="23" spans="1:15" ht="65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
-      <c r="B23" s="40" t="s">
-        <v>498</v>
+      <c r="B23" s="31" t="s">
+        <v>492</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>13</v>
@@ -4524,7 +4508,7 @@
         <v>477</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
@@ -4549,7 +4533,7 @@
         <v>479</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
@@ -4561,7 +4545,7 @@
       <c r="N24" s="15"/>
       <c r="O24" s="3"/>
     </row>
-    <row r="25" spans="1:15" ht="76" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="13" t="s">
@@ -4574,7 +4558,7 @@
         <v>477</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
@@ -4599,10 +4583,10 @@
         <v>479</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>487</v>
@@ -4617,8 +4601,8 @@
     </row>
     <row r="27" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
-      <c r="B27" s="40" t="s">
-        <v>504</v>
+      <c r="B27" s="31" t="s">
+        <v>498</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>13</v>
@@ -4630,7 +4614,7 @@
         <v>477</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
@@ -4655,7 +4639,7 @@
         <v>479</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>482</v>
@@ -4682,7 +4666,7 @@
         <v>477</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
@@ -4707,7 +4691,7 @@
         <v>479</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>

</xml_diff>